<commit_message>
working with Excel, CSV learn @Narrative
</commit_message>
<xml_diff>
--- a/src/test/resources/data/excel/usernamepassword.xlsx
+++ b/src/test/resources/data/excel/usernamepassword.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="17730"/>
+    <workbookView windowWidth="21000" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>username</t>
   </si>
@@ -32,6 +32,12 @@
   </si>
   <si>
     <t>password2</t>
+  </si>
+  <si>
+    <t>username3</t>
+  </si>
+  <si>
+    <t>password3</t>
   </si>
 </sst>
 </file>
@@ -1184,13 +1190,17 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="14.4" outlineLevelRow="3" outlineLevelCol="1"/>
+  <cols>
+    <col min="1" max="1" width="11.8055555555556" customWidth="1"/>
+    <col min="2" max="2" width="11.2314814814815" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -1216,6 +1226,14 @@
         <v>5</v>
       </c>
     </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>